<commit_message>
Add national data per surgeon
</commit_message>
<xml_diff>
--- a/clp_us_projections_ui/world-map-stats/public/National Cleft Maps_Nov2.xlsx
+++ b/clp_us_projections_ui/world-map-stats/public/National Cleft Maps_Nov2.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="191">
   <si>
     <t>State</t>
   </si>
@@ -23,6 +23,24 @@
   </si>
   <si>
     <t>2050 Predicted Clefts</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Clefts/Providers 2030</t>
+  </si>
+  <si>
+    <t>Clefts/Providers 2040</t>
+  </si>
+  <si>
+    <t>Clefts/Providers 2050</t>
+  </si>
+  <si>
+    <t>% Changes Compared to 2040</t>
+  </si>
+  <si>
+    <t>% Changes Compared to 2050</t>
   </si>
   <si>
     <t>Alabama</t>
@@ -572,8 +590,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="59" formatCode="0.0%"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -623,7 +642,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -651,6 +670,21 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
@@ -667,7 +701,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -680,7 +714,10 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -688,6 +725,15 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="59" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="59" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1740,7 +1786,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1748,8 +1794,8 @@
   <cols>
     <col min="1" max="1" width="19.8516" style="1" customWidth="1"/>
     <col min="2" max="4" width="19.3516" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.8516" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.8516" style="1" customWidth="1"/>
+    <col min="5" max="10" width="10.8516" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.8516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17" customHeight="1">
@@ -1765,757 +1811,1624 @@
       <c r="D1" t="s" s="3">
         <v>3</v>
       </c>
-      <c r="E1" s="4"/>
+      <c r="E1" t="s" s="4">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s" s="4">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s" s="4">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s" s="4">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s" s="5">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" ht="17.45" customHeight="1">
-      <c r="A2" t="s" s="5">
+      <c r="A2" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s" s="7">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s" s="7">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s" s="7">
+        <v>12</v>
+      </c>
+      <c r="E2" s="8">
+        <v>5</v>
+      </c>
+      <c r="F2" s="8">
+        <v>25</v>
+      </c>
+      <c r="G2" s="8">
+        <v>25</v>
+      </c>
+      <c r="H2" s="8">
+        <v>25</v>
+      </c>
+      <c r="I2" s="9">
+        <v>-0.001</v>
+      </c>
+      <c r="J2" s="10">
+        <v>-0.008</v>
+      </c>
+    </row>
+    <row r="3" ht="17.45" customHeight="1">
+      <c r="A3" t="s" s="6">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s" s="7">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s" s="7">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s" s="7">
+        <v>16</v>
+      </c>
+      <c r="E3" s="8">
+        <v>3</v>
+      </c>
+      <c r="F3" s="8">
+        <v>7</v>
+      </c>
+      <c r="G3" s="8">
+        <v>7</v>
+      </c>
+      <c r="H3" s="8">
+        <v>7</v>
+      </c>
+      <c r="I3" s="9">
+        <v>-0.044</v>
+      </c>
+      <c r="J3" s="10">
+        <v>-0.061</v>
+      </c>
+    </row>
+    <row r="4" ht="17.45" customHeight="1">
+      <c r="A4" t="s" s="6">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s" s="7">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s" s="7">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s" s="7">
+        <v>20</v>
+      </c>
+      <c r="E4" s="8">
+        <v>8</v>
+      </c>
+      <c r="F4" s="8">
+        <v>24</v>
+      </c>
+      <c r="G4" s="8">
+        <v>25</v>
+      </c>
+      <c r="H4" s="8">
+        <v>26</v>
+      </c>
+      <c r="I4" s="9">
+        <v>0.043</v>
+      </c>
+      <c r="J4" s="10">
+        <v>0.097</v>
+      </c>
+    </row>
+    <row r="5" ht="17.45" customHeight="1">
+      <c r="A5" t="s" s="6">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s" s="7">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s" s="7">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s" s="7">
+        <v>24</v>
+      </c>
+      <c r="E5" s="8">
+        <v>11</v>
+      </c>
+      <c r="F5" s="8">
+        <v>7</v>
+      </c>
+      <c r="G5" s="8">
+        <v>7</v>
+      </c>
+      <c r="H5" s="8">
+        <v>7</v>
+      </c>
+      <c r="I5" s="9">
+        <v>-0.022</v>
+      </c>
+      <c r="J5" s="10">
+        <v>-0.041</v>
+      </c>
+    </row>
+    <row r="6" ht="17.45" customHeight="1">
+      <c r="A6" t="s" s="6">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s" s="7">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s" s="7">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s" s="7">
+        <v>28</v>
+      </c>
+      <c r="E6" s="8">
+        <v>75</v>
+      </c>
+      <c r="F6" s="8">
+        <v>13</v>
+      </c>
+      <c r="G6" s="8">
+        <v>13</v>
+      </c>
+      <c r="H6" s="8">
+        <v>13</v>
+      </c>
+      <c r="I6" s="9">
+        <v>-0.028</v>
+      </c>
+      <c r="J6" s="10">
+        <v>-0.035</v>
+      </c>
+    </row>
+    <row r="7" ht="17.45" customHeight="1">
+      <c r="A7" t="s" s="6">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s" s="7">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s" s="7">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s" s="7">
+        <v>32</v>
+      </c>
+      <c r="E7" s="8">
+        <v>22</v>
+      </c>
+      <c r="F7" s="8">
+        <v>7</v>
+      </c>
+      <c r="G7" s="8">
+        <v>8</v>
+      </c>
+      <c r="H7" s="8">
+        <v>8</v>
+      </c>
+      <c r="I7" s="9">
+        <v>0.062</v>
+      </c>
+      <c r="J7" s="10">
+        <v>0.151</v>
+      </c>
+    </row>
+    <row r="8" ht="17.45" customHeight="1">
+      <c r="A8" t="s" s="6">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s" s="7">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s" s="7">
+        <v>35</v>
+      </c>
+      <c r="D8" t="s" s="7">
+        <v>36</v>
+      </c>
+      <c r="E8" s="8">
+        <v>12</v>
+      </c>
+      <c r="F8" s="8">
+        <v>7</v>
+      </c>
+      <c r="G8" s="8">
+        <v>6</v>
+      </c>
+      <c r="H8" s="8">
+        <v>6</v>
+      </c>
+      <c r="I8" s="9">
+        <v>-0.058</v>
+      </c>
+      <c r="J8" s="10">
+        <v>-0.121</v>
+      </c>
+    </row>
+    <row r="9" ht="17.45" customHeight="1">
+      <c r="A9" t="s" s="6">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s" s="7">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s" s="7">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s" s="7">
+        <v>40</v>
+      </c>
+      <c r="E9" s="8">
         <v>4</v>
       </c>
-      <c r="B2" t="s" s="6">
+      <c r="F9" s="8">
+        <v>3</v>
+      </c>
+      <c r="G9" s="8">
+        <v>4</v>
+      </c>
+      <c r="H9" s="8">
+        <v>4</v>
+      </c>
+      <c r="I9" s="9">
+        <v>0.043</v>
+      </c>
+      <c r="J9" s="10">
+        <v>0.097</v>
+      </c>
+    </row>
+    <row r="10" ht="17.45" customHeight="1">
+      <c r="A10" t="s" s="6">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s" s="7">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s" s="7">
+        <v>43</v>
+      </c>
+      <c r="D10" t="s" s="7">
+        <v>44</v>
+      </c>
+      <c r="E10" s="8">
+        <v>7</v>
+      </c>
+      <c r="F10" s="8">
+        <v>14</v>
+      </c>
+      <c r="G10" s="8">
+        <v>15</v>
+      </c>
+      <c r="H10" s="8">
+        <v>16</v>
+      </c>
+      <c r="I10" s="9">
+        <v>0.078</v>
+      </c>
+      <c r="J10" s="10">
+        <v>0.173</v>
+      </c>
+    </row>
+    <row r="11" ht="17.45" customHeight="1">
+      <c r="A11" t="s" s="6">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s" s="7">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s" s="7">
+        <v>47</v>
+      </c>
+      <c r="D11" t="s" s="7">
+        <v>48</v>
+      </c>
+      <c r="E11" s="8">
+        <v>36</v>
+      </c>
+      <c r="F11" s="8">
+        <v>21</v>
+      </c>
+      <c r="G11" s="8">
+        <v>22</v>
+      </c>
+      <c r="H11" s="8">
+        <v>23</v>
+      </c>
+      <c r="I11" s="9">
+        <v>0.043</v>
+      </c>
+      <c r="J11" s="10">
+        <v>0.08699999999999999</v>
+      </c>
+    </row>
+    <row r="12" ht="17.45" customHeight="1">
+      <c r="A12" t="s" s="6">
+        <v>49</v>
+      </c>
+      <c r="B12" t="s" s="7">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s" s="7">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s" s="7">
+        <v>51</v>
+      </c>
+      <c r="E12" s="8">
+        <v>14</v>
+      </c>
+      <c r="F12" s="8">
+        <v>3</v>
+      </c>
+      <c r="G12" s="8">
+        <v>3</v>
+      </c>
+      <c r="H12" s="8">
+        <v>3</v>
+      </c>
+      <c r="I12" s="9">
+        <v>0.001</v>
+      </c>
+      <c r="J12" s="10">
+        <v>0.014</v>
+      </c>
+    </row>
+    <row r="13" ht="17.45" customHeight="1">
+      <c r="A13" t="s" s="6">
+        <v>52</v>
+      </c>
+      <c r="B13" t="s" s="7">
+        <v>53</v>
+      </c>
+      <c r="C13" t="s" s="7">
+        <v>54</v>
+      </c>
+      <c r="D13" t="s" s="7">
+        <v>55</v>
+      </c>
+      <c r="E13" s="8">
+        <v>11</v>
+      </c>
+      <c r="F13" s="8">
+        <v>19</v>
+      </c>
+      <c r="G13" s="8">
+        <v>21</v>
+      </c>
+      <c r="H13" s="8">
+        <v>24</v>
+      </c>
+      <c r="I13" s="9">
+        <v>0.112</v>
+      </c>
+      <c r="J13" s="10">
+        <v>0.234</v>
+      </c>
+    </row>
+    <row r="14" ht="17.45" customHeight="1">
+      <c r="A14" t="s" s="6">
+        <v>56</v>
+      </c>
+      <c r="B14" t="s" s="7">
+        <v>57</v>
+      </c>
+      <c r="C14" t="s" s="7">
+        <v>58</v>
+      </c>
+      <c r="D14" t="s" s="7">
+        <v>59</v>
+      </c>
+      <c r="E14" s="8">
+        <v>3</v>
+      </c>
+      <c r="F14" s="8">
+        <v>8</v>
+      </c>
+      <c r="G14" s="8">
+        <v>8</v>
+      </c>
+      <c r="H14" s="8">
+        <v>7</v>
+      </c>
+      <c r="I14" s="9">
+        <v>-0.07000000000000001</v>
+      </c>
+      <c r="J14" s="10">
+        <v>-0.132</v>
+      </c>
+    </row>
+    <row r="15" ht="17.45" customHeight="1">
+      <c r="A15" t="s" s="6">
+        <v>60</v>
+      </c>
+      <c r="B15" t="s" s="7">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s" s="7">
+        <v>62</v>
+      </c>
+      <c r="D15" t="s" s="7">
+        <v>63</v>
+      </c>
+      <c r="E15" s="8">
+        <v>36</v>
+      </c>
+      <c r="F15" s="8">
+        <v>60</v>
+      </c>
+      <c r="G15" s="8">
+        <v>60</v>
+      </c>
+      <c r="H15" s="8">
+        <v>60</v>
+      </c>
+      <c r="I15" s="9">
+        <v>-0.007</v>
+      </c>
+      <c r="J15" s="10">
+        <v>-0.012</v>
+      </c>
+    </row>
+    <row r="16" ht="17.45" customHeight="1">
+      <c r="A16" t="s" s="6">
+        <v>64</v>
+      </c>
+      <c r="B16" t="s" s="7">
+        <v>65</v>
+      </c>
+      <c r="C16" t="s" s="7">
+        <v>65</v>
+      </c>
+      <c r="D16" t="s" s="7">
+        <v>66</v>
+      </c>
+      <c r="E16" s="8">
+        <v>3</v>
+      </c>
+      <c r="F16" s="8">
+        <v>14</v>
+      </c>
+      <c r="G16" s="8">
+        <v>14</v>
+      </c>
+      <c r="H16" s="8">
+        <v>14</v>
+      </c>
+      <c r="I16" s="9">
+        <v>-0.005</v>
+      </c>
+      <c r="J16" s="10">
+        <v>-0.004</v>
+      </c>
+    </row>
+    <row r="17" ht="17.45" customHeight="1">
+      <c r="A17" t="s" s="6">
+        <v>67</v>
+      </c>
+      <c r="B17" t="s" s="7">
+        <v>68</v>
+      </c>
+      <c r="C17" t="s" s="7">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s" s="7">
+        <v>69</v>
+      </c>
+      <c r="E17" s="8">
+        <v>6</v>
+      </c>
+      <c r="F17" s="8">
+        <v>8</v>
+      </c>
+      <c r="G17" s="8">
+        <v>8</v>
+      </c>
+      <c r="H17" s="8">
+        <v>8</v>
+      </c>
+      <c r="I17" s="9">
+        <v>-0.024</v>
+      </c>
+      <c r="J17" s="10">
+        <v>-0.046</v>
+      </c>
+    </row>
+    <row r="18" ht="17.45" customHeight="1">
+      <c r="A18" t="s" s="6">
+        <v>70</v>
+      </c>
+      <c r="B18" t="s" s="7">
+        <v>71</v>
+      </c>
+      <c r="C18" t="s" s="7">
+        <v>72</v>
+      </c>
+      <c r="D18" t="s" s="7">
+        <v>73</v>
+      </c>
+      <c r="E18" s="8">
+        <v>10</v>
+      </c>
+      <c r="F18" s="8">
+        <v>39</v>
+      </c>
+      <c r="G18" s="8">
+        <v>38</v>
+      </c>
+      <c r="H18" s="8">
+        <v>38</v>
+      </c>
+      <c r="I18" s="9">
+        <v>-0.008</v>
+      </c>
+      <c r="J18" s="10">
+        <v>-0.017</v>
+      </c>
+    </row>
+    <row r="19" ht="17.45" customHeight="1">
+      <c r="A19" t="s" s="6">
+        <v>74</v>
+      </c>
+      <c r="B19" t="s" s="7">
+        <v>75</v>
+      </c>
+      <c r="C19" t="s" s="7">
+        <v>76</v>
+      </c>
+      <c r="D19" t="s" s="7">
+        <v>77</v>
+      </c>
+      <c r="E19" s="8">
+        <v>3</v>
+      </c>
+      <c r="F19" s="8">
+        <v>12</v>
+      </c>
+      <c r="G19" s="8">
+        <v>12</v>
+      </c>
+      <c r="H19" s="8">
+        <v>12</v>
+      </c>
+      <c r="I19" s="9">
+        <v>-0.034</v>
+      </c>
+      <c r="J19" s="10">
+        <v>-0.057</v>
+      </c>
+    </row>
+    <row r="20" ht="17.45" customHeight="1">
+      <c r="A20" t="s" s="6">
+        <v>78</v>
+      </c>
+      <c r="B20" t="s" s="7">
+        <v>79</v>
+      </c>
+      <c r="C20" t="s" s="7">
+        <v>80</v>
+      </c>
+      <c r="D20" t="s" s="7">
+        <v>39</v>
+      </c>
+      <c r="E20" s="8">
+        <v>10</v>
+      </c>
+      <c r="F20" s="8">
+        <v>7</v>
+      </c>
+      <c r="G20" s="8">
+        <v>6</v>
+      </c>
+      <c r="H20" s="8">
+        <v>6</v>
+      </c>
+      <c r="I20" s="9">
+        <v>-0.053</v>
+      </c>
+      <c r="J20" s="10">
+        <v>-0.08</v>
+      </c>
+    </row>
+    <row r="21" ht="17.45" customHeight="1">
+      <c r="A21" t="s" s="6">
+        <v>81</v>
+      </c>
+      <c r="B21" t="s" s="7">
+        <v>82</v>
+      </c>
+      <c r="C21" t="s" s="7">
+        <v>30</v>
+      </c>
+      <c r="D21" t="s" s="7">
+        <v>83</v>
+      </c>
+      <c r="E21" s="8">
+        <v>4</v>
+      </c>
+      <c r="F21" s="8">
+        <v>23</v>
+      </c>
+      <c r="G21" s="8">
+        <v>23</v>
+      </c>
+      <c r="H21" s="8">
+        <v>23</v>
+      </c>
+      <c r="I21" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="J21" s="10">
+        <v>0.021</v>
+      </c>
+    </row>
+    <row r="22" ht="17.45" customHeight="1">
+      <c r="A22" t="s" s="6">
+        <v>84</v>
+      </c>
+      <c r="B22" t="s" s="7">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s" s="7">
+        <v>30</v>
+      </c>
+      <c r="D22" t="s" s="7">
+        <v>85</v>
+      </c>
+      <c r="E22" s="8">
+        <v>7</v>
+      </c>
+      <c r="F22" s="8">
+        <v>7</v>
+      </c>
+      <c r="G22" s="8">
+        <v>7</v>
+      </c>
+      <c r="H22" s="8">
+        <v>7</v>
+      </c>
+      <c r="I22" s="9">
+        <v>-0.001</v>
+      </c>
+      <c r="J22" s="10">
+        <v>0.003</v>
+      </c>
+    </row>
+    <row r="23" ht="17.45" customHeight="1">
+      <c r="A23" t="s" s="6">
+        <v>86</v>
+      </c>
+      <c r="B23" t="s" s="7">
+        <v>87</v>
+      </c>
+      <c r="C23" t="s" s="7">
+        <v>88</v>
+      </c>
+      <c r="D23" t="s" s="7">
+        <v>89</v>
+      </c>
+      <c r="E23" s="8">
+        <v>23</v>
+      </c>
+      <c r="F23" s="8">
+        <v>24</v>
+      </c>
+      <c r="G23" s="8">
+        <v>22</v>
+      </c>
+      <c r="H23" s="8">
+        <v>22</v>
+      </c>
+      <c r="I23" s="9">
+        <v>-0.054</v>
+      </c>
+      <c r="J23" s="10">
+        <v>-0.092</v>
+      </c>
+    </row>
+    <row r="24" ht="17.45" customHeight="1">
+      <c r="A24" t="s" s="6">
+        <v>90</v>
+      </c>
+      <c r="B24" t="s" s="7">
+        <v>91</v>
+      </c>
+      <c r="C24" t="s" s="7">
+        <v>92</v>
+      </c>
+      <c r="D24" t="s" s="7">
+        <v>93</v>
+      </c>
+      <c r="E24" s="8">
+        <v>10</v>
+      </c>
+      <c r="F24" s="8">
+        <v>10</v>
+      </c>
+      <c r="G24" s="8">
+        <v>10</v>
+      </c>
+      <c r="H24" s="8">
+        <v>11</v>
+      </c>
+      <c r="I24" s="9">
+        <v>0.018</v>
+      </c>
+      <c r="J24" s="10">
+        <v>0.043</v>
+      </c>
+    </row>
+    <row r="25" ht="17.45" customHeight="1">
+      <c r="A25" t="s" s="6">
+        <v>94</v>
+      </c>
+      <c r="B25" t="s" s="7">
+        <v>95</v>
+      </c>
+      <c r="C25" t="s" s="7">
+        <v>96</v>
+      </c>
+      <c r="D25" t="s" s="7">
+        <v>97</v>
+      </c>
+      <c r="E25" s="8">
+        <v>15</v>
+      </c>
+      <c r="F25" s="8">
+        <v>9</v>
+      </c>
+      <c r="G25" s="8">
+        <v>9</v>
+      </c>
+      <c r="H25" s="8">
+        <v>8</v>
+      </c>
+      <c r="I25" s="9">
+        <v>-0.065</v>
+      </c>
+      <c r="J25" s="10">
+        <v>-0.122</v>
+      </c>
+    </row>
+    <row r="26" ht="17.45" customHeight="1">
+      <c r="A26" t="s" s="6">
+        <v>98</v>
+      </c>
+      <c r="B26" t="s" s="7">
+        <v>99</v>
+      </c>
+      <c r="C26" t="s" s="7">
+        <v>100</v>
+      </c>
+      <c r="D26" t="s" s="7">
+        <v>101</v>
+      </c>
+      <c r="E26" s="8">
+        <v>8</v>
+      </c>
+      <c r="F26" s="8">
+        <v>26</v>
+      </c>
+      <c r="G26" s="8">
+        <v>25</v>
+      </c>
+      <c r="H26" s="8">
+        <v>25</v>
+      </c>
+      <c r="I26" s="9">
+        <v>-0.032</v>
+      </c>
+      <c r="J26" s="10">
+        <v>-0.057</v>
+      </c>
+    </row>
+    <row r="27" ht="17.45" customHeight="1">
+      <c r="A27" t="s" s="6">
+        <v>102</v>
+      </c>
+      <c r="B27" t="s" s="7">
+        <v>103</v>
+      </c>
+      <c r="C27" t="s" s="7">
+        <v>104</v>
+      </c>
+      <c r="D27" t="s" s="7">
+        <v>105</v>
+      </c>
+      <c r="E27" s="8">
+        <v>6</v>
+      </c>
+      <c r="F27" s="8">
+        <v>28</v>
+      </c>
+      <c r="G27" s="8">
+        <v>29</v>
+      </c>
+      <c r="H27" s="8">
+        <v>30</v>
+      </c>
+      <c r="I27" s="9">
+        <v>0.028</v>
+      </c>
+      <c r="J27" s="10">
+        <v>0.079</v>
+      </c>
+    </row>
+    <row r="28" ht="17.45" customHeight="1">
+      <c r="A28" t="s" s="6">
+        <v>106</v>
+      </c>
+      <c r="B28" t="s" s="7">
+        <v>107</v>
+      </c>
+      <c r="C28" t="s" s="7">
+        <v>108</v>
+      </c>
+      <c r="D28" t="s" s="7">
+        <v>109</v>
+      </c>
+      <c r="E28" s="8">
+        <v>1</v>
+      </c>
+      <c r="F28" s="8">
+        <v>7</v>
+      </c>
+      <c r="G28" s="8">
+        <v>7</v>
+      </c>
+      <c r="H28" s="8">
+        <v>8</v>
+      </c>
+      <c r="I28" s="9">
+        <v>0.024</v>
+      </c>
+      <c r="J28" s="10">
+        <v>0.051</v>
+      </c>
+    </row>
+    <row r="29" ht="17.45" customHeight="1">
+      <c r="A29" t="s" s="6">
+        <v>110</v>
+      </c>
+      <c r="B29" t="s" s="7">
+        <v>65</v>
+      </c>
+      <c r="C29" t="s" s="7">
+        <v>111</v>
+      </c>
+      <c r="D29" t="s" s="7">
+        <v>112</v>
+      </c>
+      <c r="E29" s="8">
+        <v>8</v>
+      </c>
+      <c r="F29" s="8">
+        <v>28</v>
+      </c>
+      <c r="G29" s="8">
+        <v>31</v>
+      </c>
+      <c r="H29" s="8">
+        <v>33</v>
+      </c>
+      <c r="I29" s="9">
+        <v>0.08400000000000001</v>
+      </c>
+      <c r="J29" s="10">
+        <v>0.175</v>
+      </c>
+    </row>
+    <row r="30" ht="17.45" customHeight="1">
+      <c r="A30" t="s" s="6">
+        <v>113</v>
+      </c>
+      <c r="B30" t="s" s="7">
+        <v>103</v>
+      </c>
+      <c r="C30" t="s" s="7">
+        <v>114</v>
+      </c>
+      <c r="D30" t="s" s="7">
+        <v>40</v>
+      </c>
+      <c r="E30" s="8">
+        <v>3</v>
+      </c>
+      <c r="F30" s="8">
+        <v>4</v>
+      </c>
+      <c r="G30" s="8">
+        <v>4</v>
+      </c>
+      <c r="H30" s="8">
+        <v>4</v>
+      </c>
+      <c r="I30" s="9">
+        <v>-0.043</v>
+      </c>
+      <c r="J30" s="10">
+        <v>-0.068</v>
+      </c>
+    </row>
+    <row r="31" ht="17.45" customHeight="1">
+      <c r="A31" t="s" s="6">
+        <v>115</v>
+      </c>
+      <c r="B31" t="s" s="7">
+        <v>116</v>
+      </c>
+      <c r="C31" t="s" s="7">
+        <v>117</v>
+      </c>
+      <c r="D31" t="s" s="7">
+        <v>118</v>
+      </c>
+      <c r="E31" s="8">
+        <v>7</v>
+      </c>
+      <c r="F31" s="8">
+        <v>16</v>
+      </c>
+      <c r="G31" s="8">
+        <v>16</v>
+      </c>
+      <c r="H31" s="8">
+        <v>16</v>
+      </c>
+      <c r="I31" s="9">
+        <v>-0.002</v>
+      </c>
+      <c r="J31" s="10">
+        <v>-0.014</v>
+      </c>
+    </row>
+    <row r="32" ht="17.45" customHeight="1">
+      <c r="A32" t="s" s="6">
+        <v>119</v>
+      </c>
+      <c r="B32" t="s" s="7">
+        <v>120</v>
+      </c>
+      <c r="C32" t="s" s="7">
+        <v>121</v>
+      </c>
+      <c r="D32" t="s" s="7">
+        <v>122</v>
+      </c>
+      <c r="E32" s="8">
+        <v>14</v>
+      </c>
+      <c r="F32" s="8">
+        <v>8</v>
+      </c>
+      <c r="G32" s="8">
+        <v>7</v>
+      </c>
+      <c r="H32" s="8">
+        <v>7</v>
+      </c>
+      <c r="I32" s="9">
+        <v>-0.053</v>
+      </c>
+      <c r="J32" s="10">
+        <v>-0.08500000000000001</v>
+      </c>
+    </row>
+    <row r="33" ht="17.45" customHeight="1">
+      <c r="A33" t="s" s="6">
+        <v>123</v>
+      </c>
+      <c r="B33" t="s" s="7">
+        <v>124</v>
+      </c>
+      <c r="C33" t="s" s="7">
+        <v>125</v>
+      </c>
+      <c r="D33" t="s" s="7">
+        <v>126</v>
+      </c>
+      <c r="E33" s="8">
+        <v>7</v>
+      </c>
+      <c r="F33" s="8">
+        <v>13</v>
+      </c>
+      <c r="G33" s="8">
+        <v>12</v>
+      </c>
+      <c r="H33" s="8">
+        <v>12</v>
+      </c>
+      <c r="I33" s="9">
+        <v>-0.035</v>
+      </c>
+      <c r="J33" s="10">
+        <v>-0.056</v>
+      </c>
+    </row>
+    <row r="34" ht="17.45" customHeight="1">
+      <c r="A34" t="s" s="6">
+        <v>127</v>
+      </c>
+      <c r="B34" t="s" s="7">
+        <v>128</v>
+      </c>
+      <c r="C34" t="s" s="7">
+        <v>129</v>
+      </c>
+      <c r="D34" t="s" s="7">
+        <v>130</v>
+      </c>
+      <c r="E34" s="8">
+        <v>38</v>
+      </c>
+      <c r="F34" s="8">
+        <v>15</v>
+      </c>
+      <c r="G34" s="8">
+        <v>15</v>
+      </c>
+      <c r="H34" s="8">
+        <v>16</v>
+      </c>
+      <c r="I34" s="9">
+        <v>0.035</v>
+      </c>
+      <c r="J34" s="10">
+        <v>0.074</v>
+      </c>
+    </row>
+    <row r="35" ht="17.45" customHeight="1">
+      <c r="A35" t="s" s="6">
+        <v>131</v>
+      </c>
+      <c r="B35" t="s" s="7">
+        <v>38</v>
+      </c>
+      <c r="C35" t="s" s="7">
+        <v>114</v>
+      </c>
+      <c r="D35" t="s" s="7">
+        <v>105</v>
+      </c>
+      <c r="E35" s="8">
+        <v>18</v>
+      </c>
+      <c r="F35" s="8">
+        <v>12</v>
+      </c>
+      <c r="G35" s="8">
+        <v>13</v>
+      </c>
+      <c r="H35" s="8">
+        <v>15</v>
+      </c>
+      <c r="I35" s="9">
+        <v>0.094</v>
+      </c>
+      <c r="J35" s="10">
+        <v>0.231</v>
+      </c>
+    </row>
+    <row r="36" ht="17.45" customHeight="1">
+      <c r="A36" t="s" s="6">
+        <v>132</v>
+      </c>
+      <c r="B36" t="s" s="7">
+        <v>133</v>
+      </c>
+      <c r="C36" t="s" s="7">
+        <v>134</v>
+      </c>
+      <c r="D36" t="s" s="7">
+        <v>135</v>
+      </c>
+      <c r="E36" s="8">
+        <v>2</v>
+      </c>
+      <c r="F36" s="8">
+        <v>10</v>
+      </c>
+      <c r="G36" s="8">
+        <v>9</v>
+      </c>
+      <c r="H36" s="8">
+        <v>9</v>
+      </c>
+      <c r="I36" s="9">
+        <v>-0.037</v>
+      </c>
+      <c r="J36" s="10">
+        <v>-0.06900000000000001</v>
+      </c>
+    </row>
+    <row r="37" ht="17.45" customHeight="1">
+      <c r="A37" t="s" s="6">
+        <v>136</v>
+      </c>
+      <c r="B37" t="s" s="7">
+        <v>137</v>
+      </c>
+      <c r="C37" t="s" s="7">
+        <v>137</v>
+      </c>
+      <c r="D37" t="s" s="7">
+        <v>138</v>
+      </c>
+      <c r="E37" s="8">
+        <v>30</v>
+      </c>
+      <c r="F37" s="8">
+        <v>37</v>
+      </c>
+      <c r="G37" s="8">
+        <v>37</v>
+      </c>
+      <c r="H37" s="8">
+        <v>37</v>
+      </c>
+      <c r="I37" s="9">
+        <v>0.002</v>
+      </c>
+      <c r="J37" s="10">
+        <v>0.006</v>
+      </c>
+    </row>
+    <row r="38" ht="17.45" customHeight="1">
+      <c r="A38" t="s" s="6">
+        <v>139</v>
+      </c>
+      <c r="B38" t="s" s="7">
+        <v>140</v>
+      </c>
+      <c r="C38" t="s" s="7">
+        <v>141</v>
+      </c>
+      <c r="D38" t="s" s="7">
+        <v>142</v>
+      </c>
+      <c r="E38" s="8">
+        <v>3</v>
+      </c>
+      <c r="F38" s="8">
+        <v>21</v>
+      </c>
+      <c r="G38" s="8">
+        <v>21</v>
+      </c>
+      <c r="H38" s="8">
+        <v>22</v>
+      </c>
+      <c r="I38" s="9">
+        <v>0.026</v>
+      </c>
+      <c r="J38" s="10">
+        <v>0.067</v>
+      </c>
+    </row>
+    <row r="39" ht="17.45" customHeight="1">
+      <c r="A39" t="s" s="6">
+        <v>143</v>
+      </c>
+      <c r="B39" t="s" s="7">
+        <v>144</v>
+      </c>
+      <c r="C39" t="s" s="7">
+        <v>145</v>
+      </c>
+      <c r="D39" t="s" s="7">
+        <v>146</v>
+      </c>
+      <c r="E39" s="8">
         <v>5</v>
       </c>
-      <c r="C2" t="s" s="6">
+      <c r="F39" s="8">
+        <v>14</v>
+      </c>
+      <c r="G39" s="8">
+        <v>13</v>
+      </c>
+      <c r="H39" s="8">
+        <v>13</v>
+      </c>
+      <c r="I39" s="9">
+        <v>-0.046</v>
+      </c>
+      <c r="J39" s="10">
+        <v>-0.073</v>
+      </c>
+    </row>
+    <row r="40" ht="17.45" customHeight="1">
+      <c r="A40" t="s" s="6">
+        <v>147</v>
+      </c>
+      <c r="B40" t="s" s="7">
+        <v>148</v>
+      </c>
+      <c r="C40" t="s" s="7">
+        <v>149</v>
+      </c>
+      <c r="D40" t="s" s="7">
+        <v>150</v>
+      </c>
+      <c r="E40" s="8">
+        <v>21</v>
+      </c>
+      <c r="F40" s="8">
         <v>5</v>
       </c>
-      <c r="D2" t="s" s="6">
+      <c r="G40" s="8">
+        <v>5</v>
+      </c>
+      <c r="H40" s="8">
+        <v>4</v>
+      </c>
+      <c r="I40" s="9">
+        <v>-0.038</v>
+      </c>
+      <c r="J40" s="10">
+        <v>-0.061</v>
+      </c>
+    </row>
+    <row r="41" ht="17.45" customHeight="1">
+      <c r="A41" t="s" s="6">
+        <v>151</v>
+      </c>
+      <c r="B41" t="s" s="7">
+        <v>152</v>
+      </c>
+      <c r="C41" t="s" s="7">
+        <v>153</v>
+      </c>
+      <c r="D41" t="s" s="7">
+        <v>154</v>
+      </c>
+      <c r="E41" s="8">
+        <v>5</v>
+      </c>
+      <c r="F41" s="8">
+        <v>43</v>
+      </c>
+      <c r="G41" s="8">
+        <v>45</v>
+      </c>
+      <c r="H41" s="8">
+        <v>48</v>
+      </c>
+      <c r="I41" s="9">
+        <v>0.047</v>
+      </c>
+      <c r="J41" s="10">
+        <v>0.107</v>
+      </c>
+    </row>
+    <row r="42" ht="17.45" customHeight="1">
+      <c r="A42" t="s" s="6">
+        <v>155</v>
+      </c>
+      <c r="B42" t="s" s="7">
+        <v>114</v>
+      </c>
+      <c r="C42" t="s" s="7">
+        <v>156</v>
+      </c>
+      <c r="D42" t="s" s="7">
+        <v>104</v>
+      </c>
+      <c r="E42" s="8">
+        <v>3</v>
+      </c>
+      <c r="F42" s="8">
+        <v>5</v>
+      </c>
+      <c r="G42" s="8">
+        <v>5</v>
+      </c>
+      <c r="H42" s="8">
         <v>6</v>
       </c>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" ht="17.45" customHeight="1">
-      <c r="A3" t="s" s="5">
+      <c r="I42" s="9">
+        <v>0.033</v>
+      </c>
+      <c r="J42" s="10">
+        <v>0.081</v>
+      </c>
+    </row>
+    <row r="43" ht="17.45" customHeight="1">
+      <c r="A43" t="s" s="6">
+        <v>157</v>
+      </c>
+      <c r="B43" t="s" s="7">
+        <v>61</v>
+      </c>
+      <c r="C43" t="s" s="7">
+        <v>158</v>
+      </c>
+      <c r="D43" t="s" s="7">
+        <v>159</v>
+      </c>
+      <c r="E43" s="8">
+        <v>5</v>
+      </c>
+      <c r="F43" s="8">
+        <v>11</v>
+      </c>
+      <c r="G43" s="8">
+        <v>11</v>
+      </c>
+      <c r="H43" s="8">
+        <v>11</v>
+      </c>
+      <c r="I43" s="9">
+        <v>0.031</v>
+      </c>
+      <c r="J43" s="10">
+        <v>0.066</v>
+      </c>
+    </row>
+    <row r="44" ht="17.45" customHeight="1">
+      <c r="A44" t="s" s="6">
+        <v>160</v>
+      </c>
+      <c r="B44" t="s" s="7">
+        <v>161</v>
+      </c>
+      <c r="C44" t="s" s="7">
+        <v>162</v>
+      </c>
+      <c r="D44" t="s" s="7">
+        <v>163</v>
+      </c>
+      <c r="E44" s="8">
+        <v>17</v>
+      </c>
+      <c r="F44" s="8">
+        <v>16</v>
+      </c>
+      <c r="G44" s="8">
+        <v>18</v>
+      </c>
+      <c r="H44" s="8">
+        <v>19</v>
+      </c>
+      <c r="I44" s="9">
+        <v>0.091</v>
+      </c>
+      <c r="J44" s="10">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="45" ht="17.45" customHeight="1">
+      <c r="A45" t="s" s="6">
+        <v>164</v>
+      </c>
+      <c r="B45" t="s" s="7">
+        <v>165</v>
+      </c>
+      <c r="C45" t="s" s="7">
+        <v>166</v>
+      </c>
+      <c r="D45" t="s" s="7">
+        <v>167</v>
+      </c>
+      <c r="E45" s="8">
+        <v>56</v>
+      </c>
+      <c r="F45" s="8">
+        <v>15</v>
+      </c>
+      <c r="G45" s="8">
+        <v>17</v>
+      </c>
+      <c r="H45" s="8">
+        <v>19</v>
+      </c>
+      <c r="I45" s="9">
+        <v>0.108</v>
+      </c>
+      <c r="J45" s="10">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="46" ht="17.45" customHeight="1">
+      <c r="A46" t="s" s="6">
+        <v>168</v>
+      </c>
+      <c r="B46" t="s" s="7">
+        <v>169</v>
+      </c>
+      <c r="C46" t="s" s="7">
+        <v>170</v>
+      </c>
+      <c r="D46" t="s" s="7">
+        <v>171</v>
+      </c>
+      <c r="E46" s="8">
+        <v>8</v>
+      </c>
+      <c r="F46" s="8">
+        <v>4</v>
+      </c>
+      <c r="G46" s="8">
+        <v>4</v>
+      </c>
+      <c r="H46" s="8">
+        <v>4</v>
+      </c>
+      <c r="I46" s="9">
+        <v>-0.051</v>
+      </c>
+      <c r="J46" s="10">
+        <v>-0.083</v>
+      </c>
+    </row>
+    <row r="47" ht="17.45" customHeight="1">
+      <c r="A47" t="s" s="6">
+        <v>172</v>
+      </c>
+      <c r="B47" t="s" s="7">
+        <v>173</v>
+      </c>
+      <c r="C47" t="s" s="7">
+        <v>174</v>
+      </c>
+      <c r="D47" t="s" s="7">
+        <v>175</v>
+      </c>
+      <c r="E47" s="8">
+        <v>3</v>
+      </c>
+      <c r="F47" s="8">
         <v>7</v>
       </c>
-      <c r="B3" t="s" s="6">
+      <c r="G47" s="8">
         <v>8</v>
       </c>
-      <c r="C3" t="s" s="6">
+      <c r="H47" s="8">
+        <v>8</v>
+      </c>
+      <c r="I47" s="9">
+        <v>0.028</v>
+      </c>
+      <c r="J47" s="10">
+        <v>0.048</v>
+      </c>
+    </row>
+    <row r="48" ht="17.45" customHeight="1">
+      <c r="A48" t="s" s="6">
+        <v>176</v>
+      </c>
+      <c r="B48" t="s" s="7">
+        <v>177</v>
+      </c>
+      <c r="C48" t="s" s="7">
+        <v>178</v>
+      </c>
+      <c r="D48" t="s" s="7">
+        <v>179</v>
+      </c>
+      <c r="E48" s="8">
+        <v>30</v>
+      </c>
+      <c r="F48" s="8">
+        <v>23</v>
+      </c>
+      <c r="G48" s="8">
+        <v>25</v>
+      </c>
+      <c r="H48" s="8">
+        <v>27</v>
+      </c>
+      <c r="I48" s="9">
+        <v>0.064</v>
+      </c>
+      <c r="J48" s="10">
+        <v>0.159</v>
+      </c>
+    </row>
+    <row r="49" ht="17.45" customHeight="1">
+      <c r="A49" t="s" s="6">
+        <v>180</v>
+      </c>
+      <c r="B49" t="s" s="7">
+        <v>181</v>
+      </c>
+      <c r="C49" t="s" s="7">
+        <v>182</v>
+      </c>
+      <c r="D49" t="s" s="7">
+        <v>183</v>
+      </c>
+      <c r="E49" s="8">
         <v>9</v>
       </c>
-      <c r="D3" t="s" s="6">
-        <v>10</v>
-      </c>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" ht="17.45" customHeight="1">
-      <c r="A4" t="s" s="5">
+      <c r="F49" s="8">
+        <v>12</v>
+      </c>
+      <c r="G49" s="8">
         <v>11</v>
       </c>
-      <c r="B4" t="s" s="6">
+      <c r="H49" s="8">
+        <v>11</v>
+      </c>
+      <c r="I49" s="9">
+        <v>-0.083</v>
+      </c>
+      <c r="J49" s="10">
+        <v>-0.154</v>
+      </c>
+    </row>
+    <row r="50" ht="17.45" customHeight="1">
+      <c r="A50" t="s" s="6">
+        <v>184</v>
+      </c>
+      <c r="B50" t="s" s="7">
+        <v>185</v>
+      </c>
+      <c r="C50" t="s" s="7">
+        <v>186</v>
+      </c>
+      <c r="D50" t="s" s="7">
+        <v>187</v>
+      </c>
+      <c r="E50" s="8">
+        <v>3</v>
+      </c>
+      <c r="F50" s="8">
         <v>12</v>
       </c>
-      <c r="C4" t="s" s="6">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s" s="6">
-        <v>14</v>
-      </c>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" ht="17.45" customHeight="1">
-      <c r="A5" t="s" s="5">
+      <c r="G50" s="8">
+        <v>11</v>
+      </c>
+      <c r="H50" s="8">
+        <v>11</v>
+      </c>
+      <c r="I50" s="9">
+        <v>-0.027</v>
+      </c>
+      <c r="J50" s="10">
+        <v>-0.043</v>
+      </c>
+    </row>
+    <row r="51" ht="17.45" customHeight="1">
+      <c r="A51" t="s" s="6">
+        <v>188</v>
+      </c>
+      <c r="B51" t="s" s="7">
+        <v>189</v>
+      </c>
+      <c r="C51" t="s" s="7">
+        <v>189</v>
+      </c>
+      <c r="D51" t="s" s="7">
+        <v>190</v>
+      </c>
+      <c r="E51" s="8">
+        <v>12</v>
+      </c>
+      <c r="F51" s="8">
         <v>15</v>
       </c>
-      <c r="B5" t="s" s="6">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s" s="6">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s" s="6">
-        <v>18</v>
-      </c>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" ht="17.45" customHeight="1">
-      <c r="A6" t="s" s="5">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s" s="6">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s" s="6">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s" s="6">
-        <v>22</v>
-      </c>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" ht="17.45" customHeight="1">
-      <c r="A7" t="s" s="5">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s" s="6">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s" s="6">
-        <v>25</v>
-      </c>
-      <c r="D7" t="s" s="6">
-        <v>26</v>
-      </c>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" ht="17.45" customHeight="1">
-      <c r="A8" t="s" s="5">
-        <v>27</v>
-      </c>
-      <c r="B8" t="s" s="6">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s" s="6">
-        <v>29</v>
-      </c>
-      <c r="D8" t="s" s="6">
-        <v>30</v>
-      </c>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" ht="17.45" customHeight="1">
-      <c r="A9" t="s" s="5">
-        <v>31</v>
-      </c>
-      <c r="B9" t="s" s="6">
-        <v>32</v>
-      </c>
-      <c r="C9" t="s" s="6">
-        <v>33</v>
-      </c>
-      <c r="D9" t="s" s="6">
-        <v>34</v>
-      </c>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" ht="17.45" customHeight="1">
-      <c r="A10" t="s" s="5">
-        <v>35</v>
-      </c>
-      <c r="B10" t="s" s="6">
-        <v>36</v>
-      </c>
-      <c r="C10" t="s" s="6">
-        <v>37</v>
-      </c>
-      <c r="D10" t="s" s="6">
-        <v>38</v>
-      </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" ht="17.45" customHeight="1">
-      <c r="A11" t="s" s="5">
-        <v>39</v>
-      </c>
-      <c r="B11" t="s" s="6">
-        <v>40</v>
-      </c>
-      <c r="C11" t="s" s="6">
-        <v>41</v>
-      </c>
-      <c r="D11" t="s" s="6">
-        <v>42</v>
-      </c>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" ht="17.45" customHeight="1">
-      <c r="A12" t="s" s="5">
-        <v>43</v>
-      </c>
-      <c r="B12" t="s" s="6">
-        <v>44</v>
-      </c>
-      <c r="C12" t="s" s="6">
-        <v>44</v>
-      </c>
-      <c r="D12" t="s" s="6">
-        <v>45</v>
-      </c>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" ht="17.45" customHeight="1">
-      <c r="A13" t="s" s="5">
-        <v>46</v>
-      </c>
-      <c r="B13" t="s" s="6">
-        <v>47</v>
-      </c>
-      <c r="C13" t="s" s="6">
-        <v>48</v>
-      </c>
-      <c r="D13" t="s" s="6">
-        <v>49</v>
-      </c>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" ht="17.45" customHeight="1">
-      <c r="A14" t="s" s="5">
-        <v>50</v>
-      </c>
-      <c r="B14" t="s" s="6">
-        <v>51</v>
-      </c>
-      <c r="C14" t="s" s="6">
-        <v>52</v>
-      </c>
-      <c r="D14" t="s" s="6">
-        <v>53</v>
-      </c>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" ht="17.45" customHeight="1">
-      <c r="A15" t="s" s="5">
-        <v>54</v>
-      </c>
-      <c r="B15" t="s" s="6">
-        <v>55</v>
-      </c>
-      <c r="C15" t="s" s="6">
-        <v>56</v>
-      </c>
-      <c r="D15" t="s" s="6">
-        <v>57</v>
-      </c>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" ht="17.45" customHeight="1">
-      <c r="A16" t="s" s="5">
-        <v>58</v>
-      </c>
-      <c r="B16" t="s" s="6">
-        <v>59</v>
-      </c>
-      <c r="C16" t="s" s="6">
-        <v>59</v>
-      </c>
-      <c r="D16" t="s" s="6">
-        <v>60</v>
-      </c>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" ht="17.45" customHeight="1">
-      <c r="A17" t="s" s="5">
-        <v>61</v>
-      </c>
-      <c r="B17" t="s" s="6">
-        <v>62</v>
-      </c>
-      <c r="C17" t="s" s="6">
-        <v>28</v>
-      </c>
-      <c r="D17" t="s" s="6">
-        <v>63</v>
-      </c>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" ht="17.45" customHeight="1">
-      <c r="A18" t="s" s="5">
-        <v>64</v>
-      </c>
-      <c r="B18" t="s" s="6">
-        <v>65</v>
-      </c>
-      <c r="C18" t="s" s="6">
-        <v>66</v>
-      </c>
-      <c r="D18" t="s" s="6">
-        <v>67</v>
-      </c>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" ht="17.45" customHeight="1">
-      <c r="A19" t="s" s="5">
-        <v>68</v>
-      </c>
-      <c r="B19" t="s" s="6">
-        <v>69</v>
-      </c>
-      <c r="C19" t="s" s="6">
-        <v>70</v>
-      </c>
-      <c r="D19" t="s" s="6">
-        <v>71</v>
-      </c>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" ht="17.45" customHeight="1">
-      <c r="A20" t="s" s="5">
-        <v>72</v>
-      </c>
-      <c r="B20" t="s" s="6">
-        <v>73</v>
-      </c>
-      <c r="C20" t="s" s="6">
-        <v>74</v>
-      </c>
-      <c r="D20" t="s" s="6">
-        <v>33</v>
-      </c>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" ht="17.45" customHeight="1">
-      <c r="A21" t="s" s="5">
-        <v>75</v>
-      </c>
-      <c r="B21" t="s" s="6">
-        <v>76</v>
-      </c>
-      <c r="C21" t="s" s="6">
-        <v>24</v>
-      </c>
-      <c r="D21" t="s" s="6">
-        <v>77</v>
-      </c>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" ht="17.45" customHeight="1">
-      <c r="A22" t="s" s="5">
-        <v>78</v>
-      </c>
-      <c r="B22" t="s" s="6">
-        <v>24</v>
-      </c>
-      <c r="C22" t="s" s="6">
-        <v>24</v>
-      </c>
-      <c r="D22" t="s" s="6">
-        <v>79</v>
-      </c>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" ht="17.45" customHeight="1">
-      <c r="A23" t="s" s="5">
-        <v>80</v>
-      </c>
-      <c r="B23" t="s" s="6">
-        <v>81</v>
-      </c>
-      <c r="C23" t="s" s="6">
-        <v>82</v>
-      </c>
-      <c r="D23" t="s" s="6">
-        <v>83</v>
-      </c>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" ht="17.45" customHeight="1">
-      <c r="A24" t="s" s="5">
-        <v>84</v>
-      </c>
-      <c r="B24" t="s" s="6">
-        <v>85</v>
-      </c>
-      <c r="C24" t="s" s="6">
-        <v>86</v>
-      </c>
-      <c r="D24" t="s" s="6">
-        <v>87</v>
-      </c>
-      <c r="E24" s="4"/>
-    </row>
-    <row r="25" ht="17.45" customHeight="1">
-      <c r="A25" t="s" s="5">
-        <v>88</v>
-      </c>
-      <c r="B25" t="s" s="6">
-        <v>89</v>
-      </c>
-      <c r="C25" t="s" s="6">
-        <v>90</v>
-      </c>
-      <c r="D25" t="s" s="6">
-        <v>91</v>
-      </c>
-      <c r="E25" s="4"/>
-    </row>
-    <row r="26" ht="17.45" customHeight="1">
-      <c r="A26" t="s" s="5">
-        <v>92</v>
-      </c>
-      <c r="B26" t="s" s="6">
-        <v>93</v>
-      </c>
-      <c r="C26" t="s" s="6">
-        <v>94</v>
-      </c>
-      <c r="D26" t="s" s="6">
-        <v>95</v>
-      </c>
-      <c r="E26" s="4"/>
-    </row>
-    <row r="27" ht="17.45" customHeight="1">
-      <c r="A27" t="s" s="5">
-        <v>96</v>
-      </c>
-      <c r="B27" t="s" s="6">
-        <v>97</v>
-      </c>
-      <c r="C27" t="s" s="6">
-        <v>98</v>
-      </c>
-      <c r="D27" t="s" s="6">
-        <v>99</v>
-      </c>
-      <c r="E27" s="4"/>
-    </row>
-    <row r="28" ht="17.45" customHeight="1">
-      <c r="A28" t="s" s="5">
-        <v>100</v>
-      </c>
-      <c r="B28" t="s" s="6">
-        <v>101</v>
-      </c>
-      <c r="C28" t="s" s="6">
-        <v>102</v>
-      </c>
-      <c r="D28" t="s" s="6">
-        <v>103</v>
-      </c>
-      <c r="E28" s="4"/>
-    </row>
-    <row r="29" ht="17.45" customHeight="1">
-      <c r="A29" t="s" s="5">
-        <v>104</v>
-      </c>
-      <c r="B29" t="s" s="6">
-        <v>59</v>
-      </c>
-      <c r="C29" t="s" s="6">
-        <v>105</v>
-      </c>
-      <c r="D29" t="s" s="6">
-        <v>106</v>
-      </c>
-      <c r="E29" s="4"/>
-    </row>
-    <row r="30" ht="17.45" customHeight="1">
-      <c r="A30" t="s" s="5">
-        <v>107</v>
-      </c>
-      <c r="B30" t="s" s="6">
-        <v>97</v>
-      </c>
-      <c r="C30" t="s" s="6">
-        <v>108</v>
-      </c>
-      <c r="D30" t="s" s="6">
-        <v>34</v>
-      </c>
-      <c r="E30" s="4"/>
-    </row>
-    <row r="31" ht="17.45" customHeight="1">
-      <c r="A31" t="s" s="5">
-        <v>109</v>
-      </c>
-      <c r="B31" t="s" s="6">
-        <v>110</v>
-      </c>
-      <c r="C31" t="s" s="6">
-        <v>111</v>
-      </c>
-      <c r="D31" t="s" s="6">
-        <v>112</v>
-      </c>
-      <c r="E31" s="4"/>
-    </row>
-    <row r="32" ht="17.45" customHeight="1">
-      <c r="A32" t="s" s="5">
-        <v>113</v>
-      </c>
-      <c r="B32" t="s" s="6">
-        <v>114</v>
-      </c>
-      <c r="C32" t="s" s="6">
-        <v>115</v>
-      </c>
-      <c r="D32" t="s" s="6">
-        <v>116</v>
-      </c>
-      <c r="E32" s="4"/>
-    </row>
-    <row r="33" ht="17.45" customHeight="1">
-      <c r="A33" t="s" s="5">
-        <v>117</v>
-      </c>
-      <c r="B33" t="s" s="6">
-        <v>118</v>
-      </c>
-      <c r="C33" t="s" s="6">
-        <v>119</v>
-      </c>
-      <c r="D33" t="s" s="6">
-        <v>120</v>
-      </c>
-      <c r="E33" s="4"/>
-    </row>
-    <row r="34" ht="17.45" customHeight="1">
-      <c r="A34" t="s" s="5">
-        <v>121</v>
-      </c>
-      <c r="B34" t="s" s="6">
-        <v>122</v>
-      </c>
-      <c r="C34" t="s" s="6">
-        <v>123</v>
-      </c>
-      <c r="D34" t="s" s="6">
-        <v>124</v>
-      </c>
-      <c r="E34" s="4"/>
-    </row>
-    <row r="35" ht="17.45" customHeight="1">
-      <c r="A35" t="s" s="5">
-        <v>125</v>
-      </c>
-      <c r="B35" t="s" s="6">
-        <v>32</v>
-      </c>
-      <c r="C35" t="s" s="6">
-        <v>108</v>
-      </c>
-      <c r="D35" t="s" s="6">
-        <v>99</v>
-      </c>
-      <c r="E35" s="4"/>
-    </row>
-    <row r="36" ht="17.45" customHeight="1">
-      <c r="A36" t="s" s="5">
-        <v>126</v>
-      </c>
-      <c r="B36" t="s" s="6">
-        <v>127</v>
-      </c>
-      <c r="C36" t="s" s="6">
-        <v>128</v>
-      </c>
-      <c r="D36" t="s" s="6">
-        <v>129</v>
-      </c>
-      <c r="E36" s="4"/>
-    </row>
-    <row r="37" ht="17.45" customHeight="1">
-      <c r="A37" t="s" s="5">
-        <v>130</v>
-      </c>
-      <c r="B37" t="s" s="6">
-        <v>131</v>
-      </c>
-      <c r="C37" t="s" s="6">
-        <v>131</v>
-      </c>
-      <c r="D37" t="s" s="6">
-        <v>132</v>
-      </c>
-      <c r="E37" s="4"/>
-    </row>
-    <row r="38" ht="17.45" customHeight="1">
-      <c r="A38" t="s" s="5">
-        <v>133</v>
-      </c>
-      <c r="B38" t="s" s="6">
-        <v>134</v>
-      </c>
-      <c r="C38" t="s" s="6">
-        <v>135</v>
-      </c>
-      <c r="D38" t="s" s="6">
-        <v>136</v>
-      </c>
-      <c r="E38" s="4"/>
-    </row>
-    <row r="39" ht="17.45" customHeight="1">
-      <c r="A39" t="s" s="5">
-        <v>137</v>
-      </c>
-      <c r="B39" t="s" s="6">
-        <v>138</v>
-      </c>
-      <c r="C39" t="s" s="6">
-        <v>139</v>
-      </c>
-      <c r="D39" t="s" s="6">
-        <v>140</v>
-      </c>
-      <c r="E39" s="4"/>
-    </row>
-    <row r="40" ht="17.45" customHeight="1">
-      <c r="A40" t="s" s="5">
-        <v>141</v>
-      </c>
-      <c r="B40" t="s" s="6">
-        <v>142</v>
-      </c>
-      <c r="C40" t="s" s="6">
-        <v>143</v>
-      </c>
-      <c r="D40" t="s" s="6">
-        <v>144</v>
-      </c>
-      <c r="E40" s="4"/>
-    </row>
-    <row r="41" ht="17.45" customHeight="1">
-      <c r="A41" t="s" s="5">
-        <v>145</v>
-      </c>
-      <c r="B41" t="s" s="6">
-        <v>146</v>
-      </c>
-      <c r="C41" t="s" s="6">
-        <v>147</v>
-      </c>
-      <c r="D41" t="s" s="6">
-        <v>148</v>
-      </c>
-      <c r="E41" s="4"/>
-    </row>
-    <row r="42" ht="17.45" customHeight="1">
-      <c r="A42" t="s" s="5">
-        <v>149</v>
-      </c>
-      <c r="B42" t="s" s="6">
-        <v>108</v>
-      </c>
-      <c r="C42" t="s" s="6">
-        <v>150</v>
-      </c>
-      <c r="D42" t="s" s="6">
-        <v>98</v>
-      </c>
-      <c r="E42" s="4"/>
-    </row>
-    <row r="43" ht="17.45" customHeight="1">
-      <c r="A43" t="s" s="5">
-        <v>151</v>
-      </c>
-      <c r="B43" t="s" s="6">
-        <v>55</v>
-      </c>
-      <c r="C43" t="s" s="6">
-        <v>152</v>
-      </c>
-      <c r="D43" t="s" s="6">
-        <v>153</v>
-      </c>
-      <c r="E43" s="4"/>
-    </row>
-    <row r="44" ht="17.45" customHeight="1">
-      <c r="A44" t="s" s="5">
-        <v>154</v>
-      </c>
-      <c r="B44" t="s" s="6">
-        <v>155</v>
-      </c>
-      <c r="C44" t="s" s="6">
-        <v>156</v>
-      </c>
-      <c r="D44" t="s" s="6">
-        <v>157</v>
-      </c>
-      <c r="E44" s="4"/>
-    </row>
-    <row r="45" ht="17.45" customHeight="1">
-      <c r="A45" t="s" s="5">
-        <v>158</v>
-      </c>
-      <c r="B45" t="s" s="6">
-        <v>159</v>
-      </c>
-      <c r="C45" t="s" s="6">
-        <v>160</v>
-      </c>
-      <c r="D45" t="s" s="6">
-        <v>161</v>
-      </c>
-      <c r="E45" s="4"/>
-    </row>
-    <row r="46" ht="17.45" customHeight="1">
-      <c r="A46" t="s" s="5">
-        <v>162</v>
-      </c>
-      <c r="B46" t="s" s="6">
-        <v>163</v>
-      </c>
-      <c r="C46" t="s" s="6">
-        <v>164</v>
-      </c>
-      <c r="D46" t="s" s="6">
-        <v>165</v>
-      </c>
-      <c r="E46" s="4"/>
-    </row>
-    <row r="47" ht="17.45" customHeight="1">
-      <c r="A47" t="s" s="5">
-        <v>166</v>
-      </c>
-      <c r="B47" t="s" s="6">
-        <v>167</v>
-      </c>
-      <c r="C47" t="s" s="6">
-        <v>168</v>
-      </c>
-      <c r="D47" t="s" s="6">
-        <v>169</v>
-      </c>
-      <c r="E47" s="4"/>
-    </row>
-    <row r="48" ht="17.45" customHeight="1">
-      <c r="A48" t="s" s="5">
-        <v>170</v>
-      </c>
-      <c r="B48" t="s" s="6">
-        <v>171</v>
-      </c>
-      <c r="C48" t="s" s="6">
-        <v>172</v>
-      </c>
-      <c r="D48" t="s" s="6">
-        <v>173</v>
-      </c>
-      <c r="E48" s="4"/>
-    </row>
-    <row r="49" ht="17.45" customHeight="1">
-      <c r="A49" t="s" s="5">
-        <v>174</v>
-      </c>
-      <c r="B49" t="s" s="6">
-        <v>175</v>
-      </c>
-      <c r="C49" t="s" s="6">
-        <v>176</v>
-      </c>
-      <c r="D49" t="s" s="6">
-        <v>177</v>
-      </c>
-      <c r="E49" s="4"/>
-    </row>
-    <row r="50" ht="17.45" customHeight="1">
-      <c r="A50" t="s" s="5">
-        <v>178</v>
-      </c>
-      <c r="B50" t="s" s="6">
-        <v>179</v>
-      </c>
-      <c r="C50" t="s" s="6">
-        <v>180</v>
-      </c>
-      <c r="D50" t="s" s="6">
-        <v>181</v>
-      </c>
-      <c r="E50" s="4"/>
-    </row>
-    <row r="51" ht="17.45" customHeight="1">
-      <c r="A51" t="s" s="5">
-        <v>182</v>
-      </c>
-      <c r="B51" t="s" s="6">
-        <v>183</v>
-      </c>
-      <c r="C51" t="s" s="6">
-        <v>183</v>
-      </c>
-      <c r="D51" t="s" s="6">
-        <v>184</v>
-      </c>
-      <c r="E51" s="4"/>
+      <c r="G51" s="8">
+        <v>1</v>
+      </c>
+      <c r="H51" s="8">
+        <v>15</v>
+      </c>
+      <c r="I51" s="9">
+        <v>-0.027</v>
+      </c>
+      <c r="J51" s="10">
+        <v>-0.042</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>